<commit_message>
Finish first cut at rule factoring spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC0174F-7FC7-443A-9A6A-7FF5A2301E54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBE5377-B5BC-4DB7-88A3-DC608703FBC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26964" yWindow="3420" windowWidth="34560" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="10788" yWindow="2916" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="101">
   <si>
     <t>DistinguishRuleIdFromRuleName</t>
   </si>
@@ -255,6 +255,87 @@
   </si>
   <si>
     <t>ProvideContextRegion</t>
+  </si>
+  <si>
+    <t>ProvideHelpUris</t>
+  </si>
+  <si>
+    <t>EmbedFileContent</t>
+  </si>
+  <si>
+    <t>SARIF2004</t>
+  </si>
+  <si>
+    <t>ReduceFileSize</t>
+  </si>
+  <si>
+    <t>EliminateLocationOnlyArtifacts</t>
+  </si>
+  <si>
+    <t>DoNotIncludeExtraIndexedObjectProperties</t>
+  </si>
+  <si>
+    <t>SARIF2005</t>
+  </si>
+  <si>
+    <t>ProvideHelpfulToolInformation</t>
+  </si>
+  <si>
+    <t>ProvideConciseToolName</t>
+  </si>
+  <si>
+    <t>ProvideToolVersion</t>
+  </si>
+  <si>
+    <t>UseNumericToolVersions</t>
+  </si>
+  <si>
+    <t>SARI2006</t>
+  </si>
+  <si>
+    <t>ProvideUsableUris</t>
+  </si>
+  <si>
+    <t>UrisShouldBeReachable</t>
+  </si>
+  <si>
+    <t>SARIF2007</t>
+  </si>
+  <si>
+    <t>ExpressPathsRelativeToReplRoot</t>
+  </si>
+  <si>
+    <t>(name?)</t>
+  </si>
+  <si>
+    <t>SARIF2008</t>
+  </si>
+  <si>
+    <t>ReferToFinalSchema</t>
+  </si>
+  <si>
+    <t>SchemaPropertyShouldBePresent</t>
+  </si>
+  <si>
+    <t>Schema</t>
+  </si>
+  <si>
+    <t>SARIF1011</t>
+  </si>
+  <si>
+    <t>SchemaPropertyMustReferToFinalSchema</t>
+  </si>
+  <si>
+    <t>ProvideSchema</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Content</t>
   </si>
 </sst>
 </file>
@@ -331,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -343,6 +424,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,15 +739,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.109375" style="1" bestFit="1" customWidth="1"/>
@@ -718,7 +800,7 @@
       </c>
       <c r="H2">
         <f>COUNTIF(F:F, "TODO")</f>
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -992,93 +1074,256 @@
         <v>28</v>
       </c>
     </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F32" s="7"/>
+    </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E34" s="1" t="s">
+      <c r="F35" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F34" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E35" s="1" t="s">
+      <c r="F36" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>9</v>
+      <c r="F37" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="D41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E40" s="1" t="s">
+      <c r="F41" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E42" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E41" s="1" t="s">
+      <c r="F42" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E43" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F41" s="4" t="s">
-        <v>9</v>
+      <c r="F43" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E51" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E52" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update rules spreadsheet per MF review.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larry\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B8D35D-EECE-4B1C-B4A6-06CA09141245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016B398E-7B68-4B04-807D-08E01A2C973E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10788" yWindow="2916" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="101">
-  <si>
-    <t>DistinguishRuleIdFromRuleName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="101">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -95,9 +92,6 @@
     <t>SARIF1004</t>
   </si>
   <si>
-    <t>UseUriBaseIdsCorrectly</t>
-  </si>
-  <si>
     <t>UriBaseIdRequiresRelativeUri</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>UriBaseIdValueMustNotContainQueryOrFragment</t>
   </si>
   <si>
-    <t>CertainUrisMustBeAbsolute</t>
-  </si>
-  <si>
     <t>UriMustBeAbsolute</t>
   </si>
   <si>
@@ -161,9 +152,6 @@
     <t>SARIF1008</t>
   </si>
   <si>
-    <t>ContextRegionMustEncloseRegion</t>
-  </si>
-  <si>
     <t>ContextRegionRequiresRegion</t>
   </si>
   <si>
@@ -188,9 +176,6 @@
     <t>SARIF1010</t>
   </si>
   <si>
-    <t>ResultMustContainConsistentRuleId</t>
-  </si>
-  <si>
     <t>Results</t>
   </si>
   <si>
@@ -203,9 +188,6 @@
     <t>SARIF2001</t>
   </si>
   <si>
-    <t>AuthorHighQualityRuleMessages</t>
-  </si>
-  <si>
     <t>Rules</t>
   </si>
   <si>
@@ -227,9 +209,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>UseMessagePropertiesEffectively</t>
-  </si>
-  <si>
     <t>Rules, Messages</t>
   </si>
   <si>
@@ -266,9 +245,6 @@
     <t>SARIF2004</t>
   </si>
   <si>
-    <t>ReduceFileSize</t>
-  </si>
-  <si>
     <t>EliminateLocationOnlyArtifacts</t>
   </si>
   <si>
@@ -290,24 +266,15 @@
     <t>UseNumericToolVersions</t>
   </si>
   <si>
-    <t>ProvideUsableUris</t>
-  </si>
-  <si>
     <t>UrisShouldBeReachable</t>
   </si>
   <si>
     <t>SARIF2007</t>
   </si>
   <si>
-    <t>(name?)</t>
-  </si>
-  <si>
     <t>SARIF2008</t>
   </si>
   <si>
-    <t>ReferToFinalSchema</t>
-  </si>
-  <si>
     <t>SchemaPropertyShouldBePresent</t>
   </si>
   <si>
@@ -317,9 +284,6 @@
     <t>SARIF1011</t>
   </si>
   <si>
-    <t>SchemaPropertyMustReferToFinalSchema</t>
-  </si>
-  <si>
     <t>ProvideSchema</t>
   </si>
   <si>
@@ -336,6 +300,42 @@
   </si>
   <si>
     <t>ExpressPathsRelativeToRepoRoot</t>
+  </si>
+  <si>
+    <t>ExpressUriBaseIdsCorrectly</t>
+  </si>
+  <si>
+    <t>PhysicalLocationPropertiesMustBeConsistent</t>
+  </si>
+  <si>
+    <t>RuleIdMustBeConsistent</t>
+  </si>
+  <si>
+    <t>AuthorHighQualityMessages</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>SARIF1012</t>
+  </si>
+  <si>
+    <t>MessagesPropertiesMustBeConsistent</t>
+  </si>
+  <si>
+    <t>Messages</t>
+  </si>
+  <si>
+    <t>CorrectNumberOfArguments</t>
+  </si>
+  <si>
+    <t>ReferenceFinalSchema</t>
+  </si>
+  <si>
+    <t>OptimizeFileSize</t>
+  </si>
+  <si>
+    <t>Not ready. Needs to be split</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -425,6 +425,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,16 +740,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -758,535 +759,551 @@
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <f>COUNTIF(F:F, "TODO")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="F10" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E14" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E15" s="8"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>28</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>28</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="F21" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E22" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="F22" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E25" s="1" t="s">
-        <v>44</v>
+      <c r="E25" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E28" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E31" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="F33" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="D37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E39" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="B41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E44" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E36" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E37" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="F44" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E45" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F45" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E46" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="F46" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E47" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="F47" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E50" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E42" s="1" t="s">
+      <c r="F50" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F42" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E43" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E44" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E45" s="1" t="s">
+      <c r="F52" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E53" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="F53" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E54" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E48" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E51" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E52" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="F54" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1294,36 +1311,56 @@
         <v>87</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>28</v>
+        <v>93</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update rules spreadsheet; add Rule Messages doc.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larry\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016B398E-7B68-4B04-807D-08E01A2C973E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A4411D-33C0-4CFD-8150-036D7C43D823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="8508" yWindow="3828" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -275,9 +275,6 @@
     <t>SARIF2008</t>
   </si>
   <si>
-    <t>SchemaPropertyShouldBePresent</t>
-  </si>
-  <si>
     <t>Schema</t>
   </si>
   <si>
@@ -320,15 +317,9 @@
     <t>SARIF1012</t>
   </si>
   <si>
-    <t>MessagesPropertiesMustBeConsistent</t>
-  </si>
-  <si>
     <t>Messages</t>
   </si>
   <si>
-    <t>CorrectNumberOfArguments</t>
-  </si>
-  <si>
     <t>ReferenceFinalSchema</t>
   </si>
   <si>
@@ -336,6 +327,24 @@
   </si>
   <si>
     <t>Not ready. Needs to be split</t>
+  </si>
+  <si>
+    <t>SARIF2009</t>
+  </si>
+  <si>
+    <t>UseConventionalSymbolicNames</t>
+  </si>
+  <si>
+    <t>UseConventionalRuleIds</t>
+  </si>
+  <si>
+    <t>UseConventionalUriBaseIdNames</t>
+  </si>
+  <si>
+    <t>SupplyCorrectNumberOfArguments</t>
+  </si>
+  <si>
+    <t>MessagePropertiesMustBeConsistent</t>
   </si>
 </sst>
 </file>
@@ -740,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,14 +803,14 @@
         <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H2">
         <f>COUNTIF(F:F, "TODO")</f>
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -865,7 +874,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -930,7 +939,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>25</v>
@@ -1006,7 +1015,7 @@
         <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>15</v>
@@ -1062,7 +1071,7 @@
         <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>15</v>
@@ -1090,19 +1099,19 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>25</v>
@@ -1113,19 +1122,19 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>8</v>
@@ -1136,7 +1145,7 @@
         <v>50</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>16</v>
@@ -1181,7 +1190,7 @@
         <v>59</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>8</v>
@@ -1198,7 +1207,7 @@
         <v>63</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>62</v>
@@ -1207,7 +1216,7 @@
         <v>8</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -1247,13 +1256,13 @@
         <v>69</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>70</v>
@@ -1278,10 +1287,10 @@
         <v>73</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>74</v>
@@ -1291,6 +1300,9 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C53" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E53" s="1" t="s">
         <v>75</v>
       </c>
@@ -1299,6 +1311,9 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C54" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E54" s="1" t="s">
         <v>76</v>
       </c>
@@ -1308,7 +1323,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>77</v>
@@ -1320,7 +1335,7 @@
         <v>13</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>8</v>
@@ -1331,13 +1346,13 @@
         <v>78</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F58" s="4" t="s">
         <v>8</v>
@@ -1348,19 +1363,44 @@
         <v>79</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E63" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish strings for 2009; add 'Message status' column.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larry\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A4411D-33C0-4CFD-8150-036D7C43D823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA991A39-FAC2-427D-AC44-106B0BB9F8F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8508" yWindow="3828" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="106">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -206,9 +206,6 @@
     <t>Checks to write:</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Rules, Messages</t>
   </si>
   <si>
@@ -345,6 +342,15 @@
   </si>
   <si>
     <t>MessagePropertiesMustBeConsistent</t>
+  </si>
+  <si>
+    <t>Code status</t>
+  </si>
+  <si>
+    <t>Message status</t>
+  </si>
+  <si>
+    <t>READY FOR REVIEW</t>
   </si>
 </sst>
 </file>
@@ -389,7 +395,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,6 +414,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -421,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -429,12 +441,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,29 +776,33 @@
     <col min="4" max="4" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="F1" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -803,10 +820,13 @@
         <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>25</v>
+        <v>91</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="H2">
         <f>COUNTIF(F:F, "TODO")</f>
@@ -829,7 +849,7 @@
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -874,7 +894,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -885,7 +905,7 @@
       <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -893,7 +913,7 @@
       <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -901,12 +921,12 @@
       <c r="E12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -914,7 +934,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="4" t="s">
@@ -922,7 +942,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E15" s="8"/>
+      <c r="E15" s="7"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -938,17 +958,17 @@
       <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -961,17 +981,17 @@
       <c r="D18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -984,38 +1004,38 @@
       <c r="D20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E21" s="8" t="s">
+      <c r="F20" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E21" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E22" s="8" t="s">
+      <c r="F21" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E22" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>15</v>
@@ -1023,22 +1043,28 @@
       <c r="D24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E25" s="8" t="s">
+      <c r="F24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E25" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -1054,24 +1080,24 @@
       <c r="E27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F27" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F28" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>15</v>
@@ -1082,59 +1108,59 @@
       <c r="E30" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F30" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E31" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F32" s="7"/>
+      <c r="F31" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F33" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F34" s="7"/>
+      <c r="F34" s="6"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>8</v>
@@ -1145,13 +1171,13 @@
         <v>50</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>53</v>
@@ -1172,7 +1198,7 @@
       <c r="E39" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1181,16 +1207,16 @@
         <v>55</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>8</v>
@@ -1198,30 +1224,30 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="F43" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E44" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>8</v>
@@ -1229,7 +1255,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E45" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>8</v>
@@ -1237,7 +1263,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E46" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>8</v>
@@ -1245,88 +1271,88 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E47" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="B49" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E50" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F49" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F50" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="F52" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C53" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C54" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E54" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>16</v>
@@ -1335,72 +1361,78 @@
         <v>13</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F58" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E62" s="1" t="s">
+      <c r="F62" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E63" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F62" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E63" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="F63" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Author messages for SARIF2002.UseMessageArguments.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB81804-CBDC-4E4E-A1B8-19666DCFFE86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8574D587-8AFA-4230-A10C-938C10758409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8508" yWindow="3828" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="106">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1221,6 +1221,9 @@
       <c r="F41" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="G41" s="9" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">

</xml_diff>

<commit_message>
Author messages for SARIF1012.MessagePropertiesMustBeConsistent.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8574D587-8AFA-4230-A10C-938C10758409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B134EE2-361D-4DCF-9D74-43C7F4765E71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8508" yWindow="3828" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="8856" yWindow="4176" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="106">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -433,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -447,7 +447,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,7 +780,7 @@
     <col min="4" max="4" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -799,7 +803,7 @@
       <c r="F1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>104</v>
       </c>
       <c r="H1" s="8" t="s">
@@ -825,7 +829,7 @@
       <c r="F2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>105</v>
       </c>
       <c r="H2">
@@ -1049,7 +1053,7 @@
       <c r="F24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="10" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1060,7 +1064,7 @@
       <c r="F25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="10" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1165,6 +1169,9 @@
       <c r="F35" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="G35" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -1221,7 +1228,7 @@
       <c r="F41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G41" s="10" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1423,7 +1430,7 @@
       <c r="F62" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G62" s="9" t="s">
+      <c r="G62" s="10" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1434,7 +1441,7 @@
       <c r="F63" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G63" s="9" t="s">
+      <c r="G63" s="10" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update rules factoring spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B134EE2-361D-4DCF-9D74-43C7F4765E71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA3E3FF-37BF-43EB-A8D6-59B1D2997E77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8856" yWindow="4176" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="109">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -351,13 +351,22 @@
   </si>
   <si>
     <t>READY FOR REVIEW</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Accept single quotes only. Validate rule metadata, not results strings.</t>
+  </si>
+  <si>
+    <t>Require 2 or more dot-separated numbers, followed by anything at all. We _don't_ validate semanticVersion, which should be a separate check in the same rule, and which in fact could have been in the schema!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,6 +398,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -433,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -452,6 +467,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,10 +798,11 @@
     <col min="5" max="5" width="54.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
@@ -806,11 +824,14 @@
       <c r="G1" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -832,12 +853,13 @@
       <c r="G2" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="12"/>
+      <c r="I2">
         <f>COUNTIF(F:F, "TODO")</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -857,7 +879,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
@@ -865,7 +887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
@@ -873,7 +895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -893,7 +915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -913,7 +935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
@@ -921,7 +943,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E12" s="1" t="s">
         <v>21</v>
       </c>
@@ -929,7 +951,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E13" s="7" t="s">
         <v>22</v>
       </c>
@@ -937,7 +959,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E14" s="7" t="s">
         <v>23</v>
       </c>
@@ -945,11 +967,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E15" s="7"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -969,10 +991,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -992,10 +1014,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -1015,7 +1037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E21" s="7" t="s">
         <v>36</v>
       </c>
@@ -1023,7 +1045,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E22" s="7" t="s">
         <v>37</v>
       </c>
@@ -1031,10 +1053,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
@@ -1056,8 +1078,9 @@
       <c r="G24" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E25" s="7" t="s">
         <v>40</v>
       </c>
@@ -1067,8 +1090,9 @@
       <c r="G25" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" s="12"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -1088,7 +1112,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E28" s="1" t="s">
         <v>45</v>
       </c>
@@ -1096,7 +1120,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -1116,7 +1140,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E31" s="1" t="s">
         <v>49</v>
       </c>
@@ -1124,10 +1148,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
@@ -1147,10 +1171,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>92</v>
       </c>
@@ -1172,8 +1196,9 @@
       <c r="G35" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H35" s="12"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
@@ -1192,8 +1217,11 @@
       <c r="F37" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H37" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E38" s="1" t="s">
         <v>52</v>
       </c>
@@ -1201,7 +1229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E39" s="1" t="s">
         <v>54</v>
       </c>
@@ -1209,7 +1237,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
@@ -1231,8 +1259,9 @@
       <c r="G41" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H41" s="12"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
@@ -1251,11 +1280,11 @@
       <c r="F43" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E44" s="1" t="s">
         <v>64</v>
       </c>
@@ -1263,7 +1292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E45" s="1" t="s">
         <v>65</v>
       </c>
@@ -1271,7 +1300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E46" s="1" t="s">
         <v>66</v>
       </c>
@@ -1279,7 +1308,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E47" s="1" t="s">
         <v>67</v>
       </c>
@@ -1287,7 +1316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
@@ -1307,7 +1336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E50" s="1" t="s">
         <v>70</v>
       </c>
@@ -1315,7 +1344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>71</v>
       </c>
@@ -1331,33 +1360,36 @@
       <c r="E52" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F52" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F52" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C53" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F53" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F53" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C54" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F54" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F54" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>85</v>
       </c>
@@ -1377,7 +1409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>77</v>
       </c>
@@ -1394,7 +1426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>78</v>
       </c>
@@ -1414,7 +1446,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>97</v>
       </c>
@@ -1433,8 +1465,9 @@
       <c r="G62" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H62" s="12"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E63" s="1" t="s">
         <v>100</v>
       </c>
@@ -1444,6 +1477,7 @@
       <c r="G63" s="10" t="s">
         <v>105</v>
       </c>
+      <c r="H63" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update rule factoring spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA3E3FF-37BF-43EB-A8D6-59B1D2997E77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6E6FE1-06FB-43B0-9233-B0AEAE58D25F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="-19236" yWindow="3228" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="110">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -203,9 +203,6 @@
     <t>SARIF2002</t>
   </si>
   <si>
-    <t>Checks to write:</t>
-  </si>
-  <si>
     <t>Rules, Messages</t>
   </si>
   <si>
@@ -360,6 +357,12 @@
   </si>
   <si>
     <t>Require 2 or more dot-separated numbers, followed by anything at all. We _don't_ validate semanticVersion, which should be a separate check in the same rule, and which in fact could have been in the schema!</t>
+  </si>
+  <si>
+    <t>IN PROGRESS</t>
+  </si>
+  <si>
+    <t>Checks still to write:</t>
   </si>
 </sst>
 </file>
@@ -410,7 +413,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,6 +438,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -448,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -467,8 +476,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,7 +798,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,7 +810,7 @@
     <col min="5" max="5" width="54.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="14" customWidth="1"/>
     <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -819,16 +831,16 @@
         <v>30</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>106</v>
+      <c r="H1" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -845,15 +857,14 @@
         <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="H2" s="12"/>
+        <v>104</v>
+      </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO")</f>
         <v>22</v>
@@ -920,7 +931,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -985,16 +996,16 @@
         <v>13</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -1014,10 +1025,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -1036,32 +1047,41 @@
       <c r="F20" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G20" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E21" s="7" t="s">
         <v>36</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G21" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E22" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G22" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>15</v>
@@ -1076,11 +1096,10 @@
         <v>25</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="H24" s="12"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E25" s="7" t="s">
         <v>40</v>
       </c>
@@ -1088,11 +1107,10 @@
         <v>8</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="H25" s="12"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -1112,7 +1130,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E28" s="1" t="s">
         <v>45</v>
       </c>
@@ -1120,12 +1138,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>15</v>
@@ -1139,77 +1157,82 @@
       <c r="F30" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G30" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E31" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G31" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="B35" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="H35" s="12"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>53</v>
@@ -1217,11 +1240,11 @@
       <c r="F37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H37" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H37" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E38" s="1" t="s">
         <v>52</v>
       </c>
@@ -1229,7 +1252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E39" s="1" t="s">
         <v>54</v>
       </c>
@@ -1237,80 +1260,79 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="H41" s="12"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="F43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E45" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E46" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E47" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E47" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>8</v>
@@ -1318,19 +1340,19 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>8</v>
@@ -1338,7 +1360,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E50" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>8</v>
@@ -1346,22 +1368,25 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="F52" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -1369,10 +1394,13 @@
         <v>16</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -1380,21 +1408,24 @@
         <v>16</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H54" s="13" t="s">
+      <c r="G54" s="12" t="s">
         <v>108</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>16</v>
@@ -1403,7 +1434,7 @@
         <v>13</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>8</v>
@@ -1411,16 +1442,16 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F58" s="4" t="s">
         <v>8</v>
@@ -1428,19 +1459,19 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>25</v>
@@ -1448,36 +1479,34 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="F62" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="H62" s="12"/>
+        <v>104</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E63" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="H63" s="12"/>
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update spreadsheet and restore lost edit to 1008 description.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6E6FE1-06FB-43B0-9233-B0AEAE58D25F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE78A801-3A17-49E4-9A5A-B4834A1DD034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19236" yWindow="3228" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="0" yWindow="3228" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -798,7 +798,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,7 +867,7 @@
       </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO")</f>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1103,8 +1103,8 @@
       <c r="E25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>8</v>
+      <c r="F25" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
Author messages for SARIF2005.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE78A801-3A17-49E4-9A5A-B4834A1DD034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7042CBA7-E519-4817-A96C-C2E5020708BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3228" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -798,7 +798,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,7 +808,7 @@
     <col min="3" max="3" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" style="14" customWidth="1"/>
     <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
@@ -866,8 +866,8 @@
         <v>104</v>
       </c>
       <c r="I2">
-        <f>COUNTIF(F:F, "TODO")</f>
-        <v>21</v>
+        <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -894,16 +894,16 @@
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>8</v>
+      <c r="F5" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>8</v>
+      <c r="F6" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -966,16 +966,16 @@
       <c r="E13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>8</v>
+      <c r="F13" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>8</v>
+      <c r="F14" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1237,8 +1237,8 @@
       <c r="E37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>8</v>
+      <c r="F37" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="H37" s="14" t="s">
         <v>106</v>
@@ -1248,8 +1248,8 @@
       <c r="E38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="4" t="s">
-        <v>8</v>
+      <c r="F38" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1385,8 +1385,8 @@
       <c r="F52" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G52" s="12" t="s">
-        <v>108</v>
+      <c r="G52" s="10" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -1399,8 +1399,8 @@
       <c r="F53" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G53" s="12" t="s">
-        <v>108</v>
+      <c r="G53" s="10" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -1413,8 +1413,8 @@
       <c r="F54" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G54" s="12" t="s">
-        <v>108</v>
+      <c r="G54" s="10" t="s">
+        <v>104</v>
       </c>
       <c r="H54" s="14" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
Update rules factoring spreadsheet. (#1936)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7042CBA7-E519-4817-A96C-C2E5020708BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9901D78D-5A39-45A2-8392-EE155AB60A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3228" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="112">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -363,6 +363,12 @@
   </si>
   <si>
     <t>Checks still to write:</t>
+  </si>
+  <si>
+    <t>Talk to MF. Eddy already has a PR for 1022 with more checks.</t>
+  </si>
+  <si>
+    <t>IN PROGRESS: EN</t>
   </si>
 </sst>
 </file>
@@ -457,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -481,6 +487,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,7 +874,7 @@
       </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -894,16 +901,16 @@
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>108</v>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>108</v>
+      <c r="F6" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1066,8 +1073,8 @@
       <c r="E22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>8</v>
+      <c r="F22" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>108</v>
@@ -1220,6 +1227,9 @@
       <c r="G35" s="10" t="s">
         <v>104</v>
       </c>
+      <c r="H35" s="15" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -1237,8 +1247,8 @@
       <c r="E37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="12" t="s">
-        <v>108</v>
+      <c r="F37" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="H37" s="14" t="s">
         <v>106</v>
@@ -1248,8 +1258,8 @@
       <c r="E38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="12" t="s">
-        <v>108</v>
+      <c r="F38" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1354,8 +1364,8 @@
       <c r="E49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F49" s="4" t="s">
-        <v>8</v>
+      <c r="F49" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -1490,8 +1500,8 @@
       <c r="E62" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F62" s="4" t="s">
-        <v>8</v>
+      <c r="F62" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>104</v>
@@ -1501,8 +1511,8 @@
       <c r="E63" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F63" s="4" t="s">
-        <v>8</v>
+      <c r="F63" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
Update version-related comment in rules spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9901D78D-5A39-45A2-8392-EE155AB60A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD7F534-3AC9-4902-BC65-D6E297374B2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="110">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -356,19 +356,13 @@
     <t>Accept single quotes only. Validate rule metadata, not results strings.</t>
   </si>
   <si>
-    <t>Require 2 or more dot-separated numbers, followed by anything at all. We _don't_ validate semanticVersion, which should be a separate check in the same rule, and which in fact could have been in the schema!</t>
-  </si>
-  <si>
     <t>IN PROGRESS</t>
   </si>
   <si>
     <t>Checks still to write:</t>
   </si>
   <si>
-    <t>Talk to MF. Eddy already has a PR for 1022 with more checks.</t>
-  </si>
-  <si>
-    <t>IN PROGRESS: EN</t>
+    <t>Require an integer, followed by anything at all. We _don't_ validate semanticVersion, which should be a separate check in the same rule, and which in fact could have been in the schema!</t>
   </si>
 </sst>
 </file>
@@ -463,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -487,7 +481,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,7 +840,7 @@
         <v>105</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -874,7 +867,7 @@
       </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -901,16 +894,16 @@
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>8</v>
+      <c r="F5" s="12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>25</v>
+      <c r="F6" s="12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1055,7 +1048,7 @@
         <v>25</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1066,18 +1059,18 @@
         <v>25</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>25</v>
+      <c r="F22" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1227,9 +1220,6 @@
       <c r="G35" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H35" s="15" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -1247,8 +1237,8 @@
       <c r="E37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="5" t="s">
-        <v>25</v>
+      <c r="F37" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="H37" s="14" t="s">
         <v>106</v>
@@ -1258,8 +1248,8 @@
       <c r="E38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>25</v>
+      <c r="F38" s="12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1364,8 +1354,8 @@
       <c r="E49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F49" s="12" t="s">
-        <v>111</v>
+      <c r="F49" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -1427,7 +1417,7 @@
         <v>104</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -1500,8 +1490,8 @@
       <c r="E62" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F62" s="12" t="s">
-        <v>111</v>
+      <c r="F62" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>104</v>
@@ -1511,8 +1501,8 @@
       <c r="E63" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F63" s="12" t="s">
-        <v>111</v>
+      <c r="F63" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
Update version-related comment in rules spreadsheet. (#1937)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9901D78D-5A39-45A2-8392-EE155AB60A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD7F534-3AC9-4902-BC65-D6E297374B2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="110">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -356,19 +356,13 @@
     <t>Accept single quotes only. Validate rule metadata, not results strings.</t>
   </si>
   <si>
-    <t>Require 2 or more dot-separated numbers, followed by anything at all. We _don't_ validate semanticVersion, which should be a separate check in the same rule, and which in fact could have been in the schema!</t>
-  </si>
-  <si>
     <t>IN PROGRESS</t>
   </si>
   <si>
     <t>Checks still to write:</t>
   </si>
   <si>
-    <t>Talk to MF. Eddy already has a PR for 1022 with more checks.</t>
-  </si>
-  <si>
-    <t>IN PROGRESS: EN</t>
+    <t>Require an integer, followed by anything at all. We _don't_ validate semanticVersion, which should be a separate check in the same rule, and which in fact could have been in the schema!</t>
   </si>
 </sst>
 </file>
@@ -463,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -487,7 +481,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,7 +840,7 @@
         <v>105</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -874,7 +867,7 @@
       </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -901,16 +894,16 @@
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>8</v>
+      <c r="F5" s="12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>25</v>
+      <c r="F6" s="12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1055,7 +1048,7 @@
         <v>25</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1066,18 +1059,18 @@
         <v>25</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>25</v>
+      <c r="F22" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1227,9 +1220,6 @@
       <c r="G35" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H35" s="15" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -1247,8 +1237,8 @@
       <c r="E37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="5" t="s">
-        <v>25</v>
+      <c r="F37" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="H37" s="14" t="s">
         <v>106</v>
@@ -1258,8 +1248,8 @@
       <c r="E38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>25</v>
+      <c r="F38" s="12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1364,8 +1354,8 @@
       <c r="E49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F49" s="12" t="s">
-        <v>111</v>
+      <c r="F49" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -1427,7 +1417,7 @@
         <v>104</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -1500,8 +1490,8 @@
       <c r="E62" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F62" s="12" t="s">
-        <v>111</v>
+      <c r="F62" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>104</v>
@@ -1511,8 +1501,8 @@
       <c r="E63" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F63" s="12" t="s">
-        <v>111</v>
+      <c r="F63" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
Update coding status on spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD7F534-3AC9-4902-BC65-D6E297374B2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9847747-FE62-48D4-9731-0297CD8434D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="112">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -363,6 +363,12 @@
   </si>
   <si>
     <t>Require an integer, followed by anything at all. We _don't_ validate semanticVersion, which should be a separate check in the same rule, and which in fact could have been in the schema!</t>
+  </si>
+  <si>
+    <t>IN PROGRESS: EN</t>
+  </si>
+  <si>
+    <t>IN PROGRESS: HK</t>
   </si>
 </sst>
 </file>
@@ -798,7 +804,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,7 +873,7 @@
       </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -902,8 +908,8 @@
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>107</v>
+      <c r="F6" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1066,8 +1072,8 @@
       <c r="E22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>8</v>
+      <c r="F22" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>107</v>
@@ -1237,8 +1243,8 @@
       <c r="E37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="12" t="s">
-        <v>107</v>
+      <c r="F37" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="H37" s="14" t="s">
         <v>106</v>
@@ -1248,8 +1254,8 @@
       <c r="E38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="12" t="s">
-        <v>107</v>
+      <c r="F38" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1354,16 +1360,16 @@
       <c r="E49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F49" s="4" t="s">
-        <v>8</v>
+      <c r="F49" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E50" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F50" s="4" t="s">
-        <v>8</v>
+      <c r="F50" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -1490,8 +1496,8 @@
       <c r="E62" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F62" s="4" t="s">
-        <v>8</v>
+      <c r="F62" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>104</v>
@@ -1501,8 +1507,8 @@
       <c r="E63" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F63" s="4" t="s">
-        <v>8</v>
+      <c r="F63" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
Update rule status spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9847747-FE62-48D4-9731-0297CD8434D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A7880A-6C3B-461B-A1D3-53793F061D67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="1752" yWindow="6792" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -803,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Standardize and add messages to SARIF1001.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A7880A-6C3B-461B-A1D3-53793F061D67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A49B2CF-2F04-407B-A0D4-F54FAC72379C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1752" yWindow="6792" windowWidth="34800" windowHeight="18684" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="2676" yWindow="2604" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="112">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -326,9 +326,6 @@
     <t>SARIF2009</t>
   </si>
   <si>
-    <t>UseConventionalSymbolicNames</t>
-  </si>
-  <si>
     <t>UseConventionalRuleIds</t>
   </si>
   <si>
@@ -365,10 +362,13 @@
     <t>Require an integer, followed by anything at all. We _don't_ validate semanticVersion, which should be a separate check in the same rule, and which in fact could have been in the schema!</t>
   </si>
   <si>
-    <t>IN PROGRESS: EN</t>
-  </si>
-  <si>
     <t>IN PROGRESS: HK</t>
+  </si>
+  <si>
+    <t>ConsiderConventionalIdentifierValues</t>
+  </si>
+  <si>
+    <t>We need to review the recommended set of names. Might disable this rule to start.</t>
   </si>
 </sst>
 </file>
@@ -463,16 +463,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -487,6 +484,22 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -814,39 +827,39 @@
     <col min="3" max="3" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="11" customWidth="1"/>
     <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>108</v>
+      <c r="H1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -865,11 +878,11 @@
       <c r="E2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>104</v>
+      <c r="F2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
@@ -892,7 +905,7 @@
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -900,15 +913,15 @@
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>107</v>
+      <c r="F5" s="13" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -928,7 +941,7 @@
       <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -948,7 +961,7 @@
       <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -956,7 +969,7 @@
       <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -964,28 +977,28 @@
       <c r="E12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E15" s="7"/>
+      <c r="E15" s="4"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1001,17 +1014,17 @@
       <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F16" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -1024,17 +1037,17 @@
       <c r="D18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F18" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -1047,42 +1060,42 @@
       <c r="D20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E21" s="7" t="s">
+      <c r="F20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="7" t="s">
+      <c r="F21" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
@@ -1095,28 +1108,31 @@
       <c r="D24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E25" s="7" t="s">
+      <c r="F24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F25" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L26" s="16"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -1132,19 +1148,19 @@
       <c r="E27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F27" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F28" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -1160,26 +1176,26 @@
       <c r="E30" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F30" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E31" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F32" s="6"/>
+      <c r="F31" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F32" s="15"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
@@ -1197,19 +1213,19 @@
       <c r="E33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F34" s="6"/>
+      <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>15</v>
@@ -1218,13 +1234,13 @@
         <v>92</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F35" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="10" t="s">
-        <v>104</v>
+      <c r="G35" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1243,18 +1259,18 @@
       <c r="E37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" s="14" t="s">
-        <v>106</v>
+      <c r="F37" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1262,7 +1278,7 @@
       <c r="E39" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1282,11 +1298,11 @@
       <c r="E41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G41" s="10" t="s">
-        <v>104</v>
+      <c r="G41" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -1305,7 +1321,7 @@
       <c r="E43" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H43" s="2" t="s">
@@ -1316,7 +1332,7 @@
       <c r="E44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1324,7 +1340,7 @@
       <c r="E45" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F45" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1332,7 +1348,7 @@
       <c r="E46" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1340,7 +1356,7 @@
       <c r="E47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F47" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1360,16 +1376,16 @@
       <c r="E49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F49" s="12" t="s">
-        <v>111</v>
+      <c r="F49" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E50" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F50" s="12" t="s">
-        <v>111</v>
+      <c r="F50" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -1388,11 +1404,11 @@
       <c r="E52" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>104</v>
+      <c r="F52" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -1402,11 +1418,11 @@
       <c r="E53" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F53" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>104</v>
+      <c r="F53" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -1416,14 +1432,14 @@
       <c r="E54" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F54" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H54" s="14" t="s">
-        <v>109</v>
+      <c r="F54" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -1442,7 +1458,7 @@
       <c r="E56" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F56" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1459,7 +1475,7 @@
       <c r="E58" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="F58" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1479,7 +1495,7 @@
       <c r="E60" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F60" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1488,30 +1504,33 @@
         <v>96</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="G62" s="10" t="s">
-        <v>104</v>
+        <v>25</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H62" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E63" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F63" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>104</v>
+        <v>25</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Provide messages for SARIF1002 (except for the RFC 8089 message).
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A49B2CF-2F04-407B-A0D4-F54FAC72379C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64951FEE-9E9F-40AF-B7FB-CD36C98FE367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="2604" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="112">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -816,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,6 +908,9 @@
       <c r="F4" s="12" t="s">
         <v>25</v>
       </c>
+      <c r="G4" s="7" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E5" s="1" t="s">
@@ -923,6 +926,9 @@
       </c>
       <c r="F6" s="12" t="s">
         <v>25</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Rename SARIF2005 to ProvideToolProperties.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64951FEE-9E9F-40AF-B7FB-CD36C98FE367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE47B0D9-8DE0-4FC0-A199-B9065B6EFA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="2604" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="113">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>We need to review the recommended set of names. Might disable this rule to start.</t>
+  </si>
+  <si>
+    <t>IN PROGRESS: LJG</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -479,7 +482,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -816,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,9 +829,9 @@
     <col min="3" max="3" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" style="13" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="10" customWidth="1"/>
     <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -855,7 +857,7 @@
       <c r="G1" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>104</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -878,7 +880,7 @@
       <c r="E2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G2" s="7" t="s">
@@ -905,7 +907,7 @@
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G4" s="7" t="s">
@@ -916,7 +918,7 @@
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>106</v>
       </c>
     </row>
@@ -924,7 +926,7 @@
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -967,7 +969,7 @@
       <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -975,7 +977,7 @@
       <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -983,7 +985,7 @@
       <c r="E12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -991,7 +993,7 @@
       <c r="E13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -999,7 +1001,7 @@
       <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1023,7 +1025,7 @@
       <c r="E16" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1046,7 +1048,7 @@
       <c r="E18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1069,33 +1071,33 @@
       <c r="E20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>106</v>
+      <c r="F20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>106</v>
+      <c r="F21" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>106</v>
+      <c r="F22" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -1117,7 +1119,7 @@
       <c r="E24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G24" s="7" t="s">
@@ -1128,7 +1130,7 @@
       <c r="E25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G25" s="7" t="s">
@@ -1136,7 +1138,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="L26" s="16"/>
+      <c r="L26" s="15"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -1154,7 +1156,7 @@
       <c r="E27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1162,7 +1164,7 @@
       <c r="E28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1182,7 +1184,7 @@
       <c r="E30" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -1193,7 +1195,7 @@
       <c r="E31" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G31" s="7" t="s">
@@ -1201,7 +1203,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F32" s="15"/>
+      <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
@@ -1219,12 +1221,12 @@
       <c r="E33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F34" s="15"/>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
@@ -1265,10 +1267,13 @@
       <c r="E37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" s="11" t="s">
+      <c r="F37" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="H37" s="10" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1276,16 +1281,22 @@
       <c r="E38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="12" t="s">
-        <v>25</v>
+      <c r="F38" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E39" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F39" s="12" t="s">
-        <v>25</v>
+      <c r="F39" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -1382,7 +1393,7 @@
       <c r="E49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F49" s="13" t="s">
+      <c r="F49" s="12" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1390,7 +1401,7 @@
       <c r="E50" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F50" s="13" t="s">
+      <c r="F50" s="12" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1410,7 +1421,7 @@
       <c r="E52" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G52" s="7" t="s">
@@ -1424,7 +1435,7 @@
       <c r="E53" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G53" s="7" t="s">
@@ -1438,13 +1449,13 @@
       <c r="E54" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G54" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H54" s="11" t="s">
+      <c r="H54" s="10" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1501,7 +1512,7 @@
       <c r="E60" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F60" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1518,13 +1529,13 @@
       <c r="E62" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F62" s="12" t="s">
+      <c r="F62" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H62" s="17" t="s">
+      <c r="H62" s="16" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1532,7 +1543,7 @@
       <c r="E63" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F63" s="12" t="s">
+      <c r="F63" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G63" s="7" t="s">

</xml_diff>

<commit_message>
Provide messages for SARIF2001; update code to populate arguments.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE47B0D9-8DE0-4FC0-A199-B9065B6EFA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C66F94-D72C-4BCA-A041-4E308AAF133A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="2604" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="113">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -248,9 +248,6 @@
     <t>SARIF2005</t>
   </si>
   <si>
-    <t>ProvideHelpfulToolInformation</t>
-  </si>
-  <si>
     <t>ProvideConciseToolName</t>
   </si>
   <si>
@@ -362,16 +359,19 @@
     <t>Require an integer, followed by anything at all. We _don't_ validate semanticVersion, which should be a separate check in the same rule, and which in fact could have been in the schema!</t>
   </si>
   <si>
-    <t>IN PROGRESS: HK</t>
-  </si>
-  <si>
     <t>ConsiderConventionalIdentifierValues</t>
   </si>
   <si>
     <t>We need to review the recommended set of names. Might disable this rule to start.</t>
   </si>
   <si>
-    <t>IN PROGRESS: LJG</t>
+    <t>ProvideToolProperties</t>
+  </si>
+  <si>
+    <t>TODO: IncludeDynamicContent applies to Markdown. Enquote might not because you can set values of with code font.</t>
+  </si>
+  <si>
+    <t>TODO: Don't include the string itself. DO include the rule id.</t>
   </si>
 </sst>
 </file>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,16 +852,16 @@
         <v>30</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>102</v>
-      </c>
       <c r="H1" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -878,17 +878,17 @@
         <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -911,7 +911,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -919,7 +919,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -930,7 +930,7 @@
         <v>25</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -958,7 +958,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -1023,7 +1023,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>25</v>
@@ -1075,7 +1075,7 @@
         <v>25</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -1086,7 +1086,7 @@
         <v>25</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -1097,7 +1097,7 @@
         <v>25</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -1108,7 +1108,7 @@
         <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>15</v>
@@ -1123,7 +1123,7 @@
         <v>25</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -1134,7 +1134,7 @@
         <v>25</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -1173,7 +1173,7 @@
         <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>15</v>
@@ -1188,7 +1188,7 @@
         <v>25</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -1199,7 +1199,7 @@
         <v>25</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -1207,19 +1207,19 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>25</v>
@@ -1230,25 +1230,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1256,7 +1256,7 @@
         <v>50</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>16</v>
@@ -1270,11 +1270,11 @@
       <c r="F37" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G37" s="12" t="s">
-        <v>112</v>
+      <c r="G37" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -1284,8 +1284,11 @@
       <c r="F38" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G38" s="12" t="s">
-        <v>112</v>
+      <c r="G38" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1295,7 +1298,10 @@
       <c r="F39" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G39" s="12" t="s">
+      <c r="G39" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H39" s="16" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1313,13 +1319,13 @@
         <v>57</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -1333,7 +1339,7 @@
         <v>61</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>60</v>
@@ -1342,7 +1348,7 @@
         <v>8</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -1382,19 +1388,19 @@
         <v>67</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F49" s="12" t="s">
-        <v>109</v>
+      <c r="F49" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -1402,7 +1408,7 @@
         <v>69</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -1410,22 +1416,22 @@
         <v>70</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F52" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -1433,13 +1439,13 @@
         <v>16</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -1447,24 +1453,24 @@
         <v>16</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>16</v>
@@ -1473,7 +1479,7 @@
         <v>13</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>8</v>
@@ -1481,16 +1487,16 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>8</v>
@@ -1498,19 +1504,19 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F60" s="11" t="s">
         <v>25</v>
@@ -1518,36 +1524,36 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F62" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E63" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F63" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Provide message strings for SARIF1006.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C66F94-D72C-4BCA-A041-4E308AAF133A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91F0078-9888-4A01-9A83-DB9CEEB95BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="2604" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="113">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1051,6 +1051,9 @@
       <c r="F18" s="11" t="s">
         <v>25</v>
       </c>
+      <c r="G18" s="7" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E19" s="4"/>

</xml_diff>

<commit_message>
Standardize and provide messages for SARIF1009.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91F0078-9888-4A01-9A83-DB9CEEB95BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEC1F2C-FC2E-4352-865B-00539FCFCC5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="2604" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="113">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -819,7 +819,7 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1162,6 +1162,9 @@
       <c r="F27" s="11" t="s">
         <v>25</v>
       </c>
+      <c r="G27" s="7" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E28" s="1" t="s">
@@ -1169,6 +1172,9 @@
       </c>
       <c r="F28" s="11" t="s">
         <v>25</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Reformat SARIF1005, update spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEC1F2C-FC2E-4352-865B-00539FCFCC5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E50A33-A4A8-4979-AD94-5EDD8A2710E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="2604" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1490,8 +1490,8 @@
       <c r="E56" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F56" s="3" t="s">
-        <v>8</v>
+      <c r="F56" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Reformat SARIF1005, update spreadsheet. (#1940)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEC1F2C-FC2E-4352-865B-00539FCFCC5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E50A33-A4A8-4979-AD94-5EDD8A2710E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="2604" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1490,8 +1490,8 @@
       <c r="E56" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F56" s="3" t="s">
-        <v>8</v>
+      <c r="F56" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Author "Principles" section. (#1941)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E50A33-A4A8-4979-AD94-5EDD8A2710E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD4A945-9B06-4026-9FE0-1E0837E32E25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="2604" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,8 +918,8 @@
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>105</v>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
More spreadsheet updates, a little document work.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ADA4C9-E3A3-4AC6-B284-9E3EF1EB06FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212DA199-51C9-4327-8F9E-C1E4217AF645}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4524" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="4128" yWindow="2256" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="124">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -386,21 +386,6 @@
     <t>EnquoteDynamicMessageContent</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Disabled by default. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TODO: disable the unit test until we can disable rules in tests.</t>
-    </r>
-  </si>
-  <si>
     <t>TODO: Applies to Markdown. Enquote might not because you can set values of with code font.</t>
   </si>
   <si>
@@ -417,6 +402,9 @@
   </si>
   <si>
     <t>TODO: REMOVE THIS. Keep the "rule ids" part.</t>
+  </si>
+  <si>
+    <t>Disabled by default.</t>
   </si>
 </sst>
 </file>
@@ -517,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -553,7 +541,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -873,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L71" sqref="L71"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -943,7 +930,7 @@
       </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -976,6 +963,9 @@
       <c r="F5" s="16" t="s">
         <v>102</v>
       </c>
+      <c r="G5" s="16" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E6" s="1" t="s">
@@ -1007,6 +997,9 @@
       <c r="F8" s="16" t="s">
         <v>102</v>
       </c>
+      <c r="G8" s="16" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1027,6 +1020,9 @@
       <c r="F10" s="11" t="s">
         <v>25</v>
       </c>
+      <c r="G10" s="17" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E11" s="1" t="s">
@@ -1035,6 +1031,9 @@
       <c r="F11" s="11" t="s">
         <v>25</v>
       </c>
+      <c r="G11" s="17" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E12" s="1" t="s">
@@ -1043,6 +1042,9 @@
       <c r="F12" s="11" t="s">
         <v>25</v>
       </c>
+      <c r="G12" s="17" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E13" s="4" t="s">
@@ -1051,6 +1053,9 @@
       <c r="F13" s="11" t="s">
         <v>25</v>
       </c>
+      <c r="G13" s="17" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E14" s="4" t="s">
@@ -1059,6 +1064,9 @@
       <c r="F14" s="11" t="s">
         <v>25</v>
       </c>
+      <c r="G14" s="17" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E15" s="4"/>
@@ -1354,7 +1362,7 @@
         <v>52</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>16</v>
@@ -1365,14 +1373,11 @@
       <c r="E40" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F40" s="18" t="s">
-        <v>121</v>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -1391,10 +1396,12 @@
       <c r="E42" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H42" s="17"/>
+      <c r="F42" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -1424,7 +1431,7 @@
         <v>8</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -1509,7 +1516,7 @@
         <v>25</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -1583,7 +1590,7 @@
         <v>91</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -1699,7 +1706,7 @@
         <v>91</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
More spreadsheet updates and document work.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212DA199-51C9-4327-8F9E-C1E4217AF645}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A56CF90-1FC9-4D88-8557-263F645905C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4128" yWindow="2256" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -930,7 +930,7 @@
       </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1396,12 +1396,10 @@
       <c r="E42" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F42" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="F42" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -1639,8 +1637,11 @@
       <c r="E63" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F63" s="3" t="s">
-        <v>8</v>
+      <c r="F63" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Remove obsolete "uriBaseId conventions" text.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5080B4-0A85-454B-953A-FF0B63D45D22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EE69A8-D2BF-4CD3-B4CD-E3A6E3B6306D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4128" yWindow="2256" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="119">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1541,6 +1541,9 @@
       <c r="F56" s="10" t="s">
         <v>24</v>
       </c>
+      <c r="G56" s="6" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">

</xml_diff>

<commit_message>
Fix doc errors; update spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EE69A8-D2BF-4CD3-B4CD-E3A6E3B6306D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C16139-8804-46B5-AA6D-64544F0F5902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4128" yWindow="2256" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="121">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -390,6 +390,12 @@
   </si>
   <si>
     <t>If region and contextRegion are both present, ask for snippets on both.</t>
+  </si>
+  <si>
+    <t>ProvideUriBaseIdForMappedTo</t>
+  </si>
+  <si>
+    <t>ExpressResultLocationsRelativeToMappedTo</t>
   </si>
 </sst>
 </file>
@@ -834,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -906,7 +912,7 @@
       </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1513,7 +1519,7 @@
         <v>15</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="F54" s="16" t="s">
         <v>113</v>
@@ -1522,194 +1528,202 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E55" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F55" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F56" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="F57" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F58" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H58" s="14"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
+      <c r="F59" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F60" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H60" s="9" t="s">
+      <c r="F61" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H61" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F61" s="1"/>
-    </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F62" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="F63" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F64" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="F65" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F66" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+      <c r="F67" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E69" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F68" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H68" s="9" t="s">
+      <c r="F69" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H69" s="9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="14"/>
-    </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="14"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E71" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F70" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G70" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H70" s="14"/>
+      <c r="F71" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H71" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update spreadsheet: last rule written!
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C16139-8804-46B5-AA6D-64544F0F5902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BE7916-5CBA-409B-B774-E596EFFDCDC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4128" yWindow="2256" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="119">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -372,12 +372,6 @@
   </si>
   <si>
     <t>ProvideMessageArguments</t>
-  </si>
-  <si>
-    <t>IN PROGRESS</t>
-  </si>
-  <si>
-    <t>Eddy</t>
   </si>
   <si>
     <t>Disabled by default.</t>
@@ -446,7 +440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,12 +465,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -490,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -521,9 +509,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -842,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +897,7 @@
       </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1420,7 +1405,7 @@
         <v>24</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -1505,7 +1490,7 @@
         <v>24</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -1519,21 +1504,18 @@
         <v>15</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F54" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>114</v>
+        <v>117</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E55" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F55" s="16" t="s">
-        <v>113</v>
+        <v>118</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -1604,7 +1586,7 @@
         <v>24</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
@@ -1693,7 +1675,7 @@
         <v>89</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Introduce SARIF1003 in spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BE7916-5CBA-409B-B774-E596EFFDCDC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B645971-8524-45BD-B0C5-B0AE29F6B92E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4128" yWindow="2256" windowWidth="39780" windowHeight="20796" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="123">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -390,6 +388,18 @@
   </si>
   <si>
     <t>ExpressResultLocationsRelativeToMappedTo</t>
+  </si>
+  <si>
+    <t>SARIF1013</t>
+  </si>
+  <si>
+    <t>ArtifactLocationPropertiesMustBeConsistent</t>
+  </si>
+  <si>
+    <t>Artifact</t>
+  </si>
+  <si>
+    <t>TODO</t>
   </si>
 </sst>
 </file>
@@ -440,7 +450,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,6 +475,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -478,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -509,6 +525,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -825,26 +844,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" style="11" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6328125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -873,7 +892,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -897,10 +916,10 @@
       </c>
       <c r="I2">
         <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -923,7 +942,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
@@ -934,7 +953,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
@@ -945,30 +964,33 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -982,7 +1004,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>24</v>
@@ -991,9 +1013,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>24</v>
@@ -1002,9 +1024,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E12" s="1" t="s">
-        <v>20</v>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E12" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>24</v>
@@ -1013,9 +1035,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>24</v>
@@ -1024,88 +1046,88 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E15" s="3"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E14" s="3"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="F15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="F17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="E19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E20" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>24</v>
@@ -1114,9 +1136,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E21" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>24</v>
@@ -1125,35 +1147,35 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="E23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E24" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>24</v>
@@ -1162,35 +1184,35 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="L26" s="13"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L25" s="13"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="E26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E27" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>24</v>
@@ -1199,32 +1221,32 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="E29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E30" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F30" s="10" t="s">
         <v>24</v>
@@ -1233,61 +1255,61 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F34" s="12"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="F32" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="E34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E35" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>24</v>
@@ -1296,55 +1318,47 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E36" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>107</v>
+        <v>13</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>80</v>
@@ -1355,19 +1369,22 @@
       <c r="G40" s="6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H40" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>80</v>
@@ -1375,229 +1392,247 @@
       <c r="F42" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H42" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G42" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F44" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E45" s="1" t="s">
+      <c r="F46" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E47" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F45" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H45" s="9" t="s">
+      <c r="F47" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H47" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E46" s="1" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E48" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="F48" s="15" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="G48" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F48" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C49" s="1" t="s">
+      <c r="F50" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C51" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F49" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C50" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="F51" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C52" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E52" s="1" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>24</v>
       </c>
+      <c r="G52" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="H52" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D54" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E54" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F54" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E55" s="1" t="s">
+      <c r="F56" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E57" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F55" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+      <c r="F57" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F57" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="F59" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H59" s="14"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="E61" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H61" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G61" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H61" s="14"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>55</v>
@@ -1611,13 +1646,22 @@
       <c r="F63" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G63" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>55</v>
@@ -1631,13 +1675,16 @@
       <c r="F65" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G65" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>55</v>
@@ -1651,19 +1698,22 @@
       <c r="F67" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G67" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>80</v>
@@ -1671,24 +1721,16 @@
       <c r="F69" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G69" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H69" s="9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="14"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G69" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>55</v>
@@ -1705,7 +1747,38 @@
       <c r="G71" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="H71" s="14"/>
+      <c r="H71" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="14"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H73" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Doc update for 2005/8/9.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780D38EE-1C30-4080-8D01-8465BA8B38DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F45E35-9692-48B0-A044-3BB1859F218B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1581,8 +1581,8 @@
       <c r="G50" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H50" s="13" t="s">
-        <v>121</v>
+      <c r="H50" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
@@ -1598,8 +1598,8 @@
       <c r="G51" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H51" s="13" t="s">
-        <v>121</v>
+      <c r="H51" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
@@ -1615,8 +1615,8 @@
       <c r="G52" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H52" s="13" t="s">
-        <v>121</v>
+      <c r="H52" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>92</v>
@@ -1710,8 +1710,8 @@
       <c r="G59" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H59" s="13" t="s">
-        <v>121</v>
+      <c r="H59" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
@@ -1733,8 +1733,8 @@
       <c r="G61" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H61" s="13" t="s">
-        <v>121</v>
+      <c r="H61" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I61" s="11"/>
     </row>

</xml_diff>

<commit_message>
Doc update for 2014/15.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F45E35-9692-48B0-A044-3BB1859F218B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AF3328-5508-4926-B777-F66E27F9CAF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1875,8 +1875,8 @@
       <c r="G71" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H71" s="13" t="s">
-        <v>121</v>
+      <c r="H71" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I71" s="6" t="s">
         <v>114</v>
@@ -1910,8 +1910,8 @@
       <c r="G73" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H73" s="13" t="s">
-        <v>121</v>
+      <c r="H73" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I73" s="11"/>
     </row>

</xml_diff>

<commit_message>
Spreadsheet update for 1004.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AF3328-5508-4926-B777-F66E27F9CAF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A243B6BD-8EFC-44F7-BA4B-DDA8C5F90BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -32,8 +32,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={63376904-47E8-4E19-B0B3-4CC82628F150}</author>
+  </authors>
+  <commentList>
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{63376904-47E8-4E19-B0B3-4CC82628F150}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    We also have to generalize the rule description for this one -- it's about all uriBaseIds, not just the ones in originalUriBaseIds.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="121">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -387,15 +405,6 @@
   </si>
   <si>
     <t>ExpressResultLocationsRelativeToMappedTo</t>
-  </si>
-  <si>
-    <t>SARIF1013</t>
-  </si>
-  <si>
-    <t>ArtifactLocationPropertiesMustBeConsistent</t>
-  </si>
-  <si>
-    <t>Artifact</t>
   </si>
   <si>
     <t>TODO</t>
@@ -551,6 +560,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Larry Golding (Myriad Consulting Inc)" id="{D924DA7C-F2B3-424C-9D13-1366042C7316}" userId="S::v-lgold@microsoft.com::9879b265-b605-48ed-ae2d-d89acc938fdf" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -848,12 +863,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G14" dT="2020-07-03T01:17:37.97" personId="{D924DA7C-F2B3-424C-9D13-1366042C7316}" id="{63376904-47E8-4E19-B0B3-4CC82628F150}">
+    <text>We also have to generalize the rule description for this one -- it's about all uriBaseIds, not just the ones in originalUriBaseIds.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -890,10 +913,10 @@
         <v>87</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>89</v>
@@ -929,7 +952,7 @@
       </c>
       <c r="J2">
         <f>COUNTIF(F:F, "TODO") + COUNTIF(F:F, "IN PROGRESS")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -991,25 +1014,25 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>119</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>121</v>
+        <v>16</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1081,96 +1104,96 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="E14" s="3"/>
-      <c r="J14" s="2"/>
+      <c r="E14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="E15" s="3"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="E16" s="3"/>
+      <c r="F16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E18" s="3"/>
+      <c r="F18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E20" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>24</v>
@@ -1184,240 +1207,228 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E22" s="3"/>
+      <c r="F22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E25" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="M25" s="10"/>
+      <c r="F25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="M26" s="10"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="F28" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E31" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F31" s="9"/>
+      <c r="F31" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F32" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F33" s="9"/>
+      <c r="F33" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E36" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>97</v>
+      <c r="F36" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -1495,10 +1506,10 @@
         <v>24</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I44" s="1"/>
     </row>
@@ -1522,10 +1533,10 @@
         <v>24</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -1536,10 +1547,10 @@
         <v>24</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>113</v>
@@ -1642,10 +1653,10 @@
         <v>24</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I54" s="6" t="s">
         <v>112</v>
@@ -1668,10 +1679,10 @@
         <v>24</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
@@ -1682,10 +1693,10 @@
         <v>24</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
@@ -1763,10 +1774,10 @@
         <v>24</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I63" s="6" t="s">
         <v>115</v>
@@ -1795,10 +1806,10 @@
         <v>24</v>
       </c>
       <c r="G65" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -1821,10 +1832,10 @@
         <v>24</v>
       </c>
       <c r="G67" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
@@ -1847,10 +1858,10 @@
         <v>24</v>
       </c>
       <c r="G69" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -1918,5 +1929,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update messages and code for SARIF1004.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A243B6BD-8EFC-44F7-BA4B-DDA8C5F90BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD4D847-A7CE-4D7E-865C-AEC5AF6CDB50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -30,24 +30,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={63376904-47E8-4E19-B0B3-4CC82628F150}</author>
-  </authors>
-  <commentList>
-    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{63376904-47E8-4E19-B0B3-4CC82628F150}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    We also have to generalize the rule description for this one -- it's about all uriBaseIds, not just the ones in originalUriBaseIds.</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -563,9 +545,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Larry Golding (Myriad Consulting Inc)" id="{D924DA7C-F2B3-424C-9D13-1366042C7316}" userId="S::v-lgold@microsoft.com::9879b265-b605-48ed-ae2d-d89acc938fdf" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -863,20 +843,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G14" dT="2020-07-03T01:17:37.97" personId="{D924DA7C-F2B3-424C-9D13-1366042C7316}" id="{63376904-47E8-4E19-B0B3-4CC82628F150}">
-    <text>We also have to generalize the rule description for this one -- it's about all uriBaseIds, not just the ones in originalUriBaseIds.</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1110,11 +1082,11 @@
       <c r="F14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>118</v>
+      <c r="G14" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -1929,6 +1901,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update messages and code for SARIF1004. (#1968)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A243B6BD-8EFC-44F7-BA4B-DDA8C5F90BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD4D847-A7CE-4D7E-865C-AEC5AF6CDB50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -30,24 +30,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={63376904-47E8-4E19-B0B3-4CC82628F150}</author>
-  </authors>
-  <commentList>
-    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{63376904-47E8-4E19-B0B3-4CC82628F150}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    We also have to generalize the rule description for this one -- it's about all uriBaseIds, not just the ones in originalUriBaseIds.</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -563,9 +545,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Larry Golding (Myriad Consulting Inc)" id="{D924DA7C-F2B3-424C-9D13-1366042C7316}" userId="S::v-lgold@microsoft.com::9879b265-b605-48ed-ae2d-d89acc938fdf" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -863,20 +843,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G14" dT="2020-07-03T01:17:37.97" personId="{D924DA7C-F2B3-424C-9D13-1366042C7316}" id="{63376904-47E8-4E19-B0B3-4CC82628F150}">
-    <text>We also have to generalize the rule description for this one -- it's about all uriBaseIds, not just the ones in originalUriBaseIds.</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1110,11 +1082,11 @@
       <c r="F14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>118</v>
+      <c r="G14" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -1929,6 +1901,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Provide messages for SARIF2003.ProvideVersionControlProvenance.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD4D847-A7CE-4D7E-865C-AEC5AF6CDB50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690D1540-BDE9-448E-A485-5EE024AEDD9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -542,10 +542,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -845,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
-  <dimension ref="A1:M73"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1403,18 +1399,47 @@
         <v>24</v>
       </c>
     </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>80</v>
@@ -1428,22 +1453,19 @@
       <c r="H40" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I40" s="6" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>80</v>
@@ -1457,22 +1479,23 @@
       <c r="H42" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="I42" s="1"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>24</v>
@@ -1483,80 +1506,87 @@
       <c r="H44" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E45" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="E46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C49" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G46" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H46" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E47" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H47" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E48" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="G48" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="H48" s="12" t="s">
-        <v>97</v>
+      <c r="E49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G49" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="C50" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>24</v>
@@ -1567,59 +1597,51 @@
       <c r="H50" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C51" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G51" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>24</v>
+      <c r="I50" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="C52" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D52" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E52" s="1" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G52" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>24</v>
+      <c r="G52" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E54" s="1" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>24</v>
@@ -1630,62 +1652,59 @@
       <c r="H54" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="I54" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C56" s="1" t="s">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E55" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G56" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H56" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D57" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="E57" s="1" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G57" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H57" s="13" t="s">
-        <v>118</v>
+      <c r="G57" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>24</v>
@@ -1696,42 +1715,51 @@
       <c r="H59" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="I59" s="11"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F60" s="1"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="D61" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="E61" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G61" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H61" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I61" s="11"/>
+      <c r="G61" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F62" s="1"/>
-      <c r="G62" s="15"/>
-      <c r="H62" s="15"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>55</v>
@@ -1751,19 +1779,13 @@
       <c r="H63" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="I63" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>55</v>
@@ -1786,10 +1808,10 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>55</v>
@@ -1812,16 +1834,16 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>80</v>
@@ -1829,19 +1851,28 @@
       <c r="F69" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G69" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H69" s="13" t="s">
-        <v>118</v>
-      </c>
+      <c r="G69" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F70" s="1"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="11"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>55</v>
@@ -1861,42 +1892,7 @@
       <c r="H71" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I71" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F72" s="1"/>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15"/>
-      <c r="I72" s="11"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G73" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H73" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I73" s="11"/>
+      <c r="I71" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Provide messages for SARIF2003.ProvideVersionControlProvenance. (#1970)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD4D847-A7CE-4D7E-865C-AEC5AF6CDB50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690D1540-BDE9-448E-A485-5EE024AEDD9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -542,10 +542,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -845,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
-  <dimension ref="A1:M73"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1403,18 +1399,47 @@
         <v>24</v>
       </c>
     </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>80</v>
@@ -1428,22 +1453,19 @@
       <c r="H40" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I40" s="6" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>80</v>
@@ -1457,22 +1479,23 @@
       <c r="H42" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="I42" s="1"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>24</v>
@@ -1483,80 +1506,87 @@
       <c r="H44" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E45" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="E46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C49" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G46" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H46" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E47" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H47" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E48" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="G48" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="H48" s="12" t="s">
-        <v>97</v>
+      <c r="E49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G49" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="C50" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>24</v>
@@ -1567,59 +1597,51 @@
       <c r="H50" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C51" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G51" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>24</v>
+      <c r="I50" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="C52" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D52" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E52" s="1" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G52" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>24</v>
+      <c r="G52" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E54" s="1" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>24</v>
@@ -1630,62 +1652,59 @@
       <c r="H54" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="I54" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C56" s="1" t="s">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E55" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G56" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H56" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D57" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="E57" s="1" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G57" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H57" s="13" t="s">
-        <v>118</v>
+      <c r="G57" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>24</v>
@@ -1696,42 +1715,51 @@
       <c r="H59" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="I59" s="11"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F60" s="1"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="D61" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="E61" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G61" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H61" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I61" s="11"/>
+      <c r="G61" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F62" s="1"/>
-      <c r="G62" s="15"/>
-      <c r="H62" s="15"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>55</v>
@@ -1751,19 +1779,13 @@
       <c r="H63" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="I63" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>55</v>
@@ -1786,10 +1808,10 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>55</v>
@@ -1812,16 +1834,16 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>80</v>
@@ -1829,19 +1851,28 @@
       <c r="F69" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G69" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H69" s="13" t="s">
-        <v>118</v>
-      </c>
+      <c r="G69" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F70" s="1"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="11"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>55</v>
@@ -1861,42 +1892,7 @@
       <c r="H71" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I71" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F72" s="1"/>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15"/>
-      <c r="I72" s="11"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G73" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H73" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I73" s="11"/>
+      <c r="I71" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Provide messages for SARIF2004.OptimizeFileSize.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690D1540-BDE9-448E-A485-5EE024AEDD9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A380A5-4A7A-49F1-B818-60623D700BC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -844,7 +844,7 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1500,11 +1500,11 @@
       <c r="F44" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G44" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>118</v>
+      <c r="G44" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -1514,11 +1514,11 @@
       <c r="F45" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H45" s="13" t="s">
-        <v>118</v>
+      <c r="G45" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Provide messages for SARIF2004.OptimizeFileSize. (#1973)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690D1540-BDE9-448E-A485-5EE024AEDD9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A380A5-4A7A-49F1-B818-60623D700BC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -844,7 +844,7 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1500,11 +1500,11 @@
       <c r="F44" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G44" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>118</v>
+      <c r="G44" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -1514,11 +1514,11 @@
       <c r="F45" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H45" s="13" t="s">
-        <v>118</v>
+      <c r="G45" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Provide messages for SARIF2006.MessagesShouldBeReachable.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A380A5-4A7A-49F1-B818-60623D700BC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38593DA7-8E77-4276-A7B9-7B962EF91EFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="3200" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -844,7 +844,7 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1620,11 +1620,11 @@
       <c r="F52" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G52" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H52" s="13" t="s">
-        <v>118</v>
+      <c r="G52" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>112</v>

</xml_diff>

<commit_message>
Provide messages for SARIF2006.MessagesShouldBeReachable. (#1974)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A380A5-4A7A-49F1-B818-60623D700BC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38593DA7-8E77-4276-A7B9-7B962EF91EFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
+    <workbookView xWindow="3200" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -844,7 +844,7 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1620,11 +1620,11 @@
       <c r="F52" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G52" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H52" s="13" t="s">
-        <v>118</v>
+      <c r="G52" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>112</v>

</xml_diff>

<commit_message>
Provide messages for SARIF2007.ExpressLocationsRelativeToRepoRoot.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38593DA7-8E77-4276-A7B9-7B962EF91EFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA19B7D5-9363-410C-87CE-A56DA19C5C14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1646,11 +1646,11 @@
       <c r="F54" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G54" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H54" s="13" t="s">
-        <v>118</v>
+      <c r="G54" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
@@ -1660,11 +1660,11 @@
       <c r="F55" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G55" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H55" s="13" t="s">
-        <v>118</v>
+      <c r="G55" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Provide messages for SARIF2007.ExpressLocationsRelativeToRepoRoot. (#1975)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38593DA7-8E77-4276-A7B9-7B962EF91EFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA19B7D5-9363-410C-87CE-A56DA19C5C14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1646,11 +1646,11 @@
       <c r="F54" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G54" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H54" s="13" t="s">
-        <v>118</v>
+      <c r="G54" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
@@ -1660,11 +1660,11 @@
       <c r="F55" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G55" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H55" s="13" t="s">
-        <v>118</v>
+      <c r="G55" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Provide messages for SARIF1012.ProvideHelpUris.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA19B7D5-9363-410C-87CE-A56DA19C5C14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C2398E-72FA-4244-AA3B-13112BDA45FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1799,11 +1799,11 @@
       <c r="F65" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G65" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H65" s="13" t="s">
-        <v>118</v>
+      <c r="G65" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Provide messages for SARIF1012.ProvideHelpUris. (#1976)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA19B7D5-9363-410C-87CE-A56DA19C5C14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C2398E-72FA-4244-AA3B-13112BDA45FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5997C-BAA7-4C98-B051-AE61EF1FF683}">
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1799,11 +1799,11 @@
       <c r="F65" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G65" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H65" s="13" t="s">
-        <v>118</v>
+      <c r="G65" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Provide messages for SARIF2013.ProvideEmbeddedFileContent.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C2398E-72FA-4244-AA3B-13112BDA45FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF296D5-B336-42A5-BDF6-97A9571E008D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -844,7 +844,7 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1825,11 +1825,11 @@
       <c r="F67" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G67" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H67" s="13" t="s">
-        <v>118</v>
+      <c r="G67" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Provide messages for SARIF2013.ProvideEmbeddedFileContent. (#1977)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C2398E-72FA-4244-AA3B-13112BDA45FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF296D5-B336-42A5-BDF6-97A9571E008D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -844,7 +844,7 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1825,11 +1825,11 @@
       <c r="F67" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G67" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H67" s="13" t="s">
-        <v>118</v>
+      <c r="G67" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Provide messages for SARIF2010.ProvideCodeSnippets.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF296D5-B336-42A5-BDF6-97A9571E008D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DD2164-FE87-4C44-8B24-B0B2E66C184C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -844,7 +844,7 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1741,11 +1741,11 @@
       <c r="F61" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G61" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H61" s="13" t="s">
-        <v>118</v>
+      <c r="G61" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I61" s="6" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
Provide messages for SARIF2010.ProvideCodeSnippets. (#1979)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF296D5-B336-42A5-BDF6-97A9571E008D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DD2164-FE87-4C44-8B24-B0B2E66C184C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -844,7 +844,7 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1741,11 +1741,11 @@
       <c r="F61" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G61" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H61" s="13" t="s">
-        <v>118</v>
+      <c r="G61" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I61" s="6" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
Provide messages for SARIF2011.ProvideContextRegion.
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DD2164-FE87-4C44-8B24-B0B2E66C184C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F7FAC9-0971-4894-927F-B3F7EA8F1BE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="120">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -387,9 +387,6 @@
   </si>
   <si>
     <t>ExpressResultLocationsRelativeToMappedTo</t>
-  </si>
-  <si>
-    <t>TODO</t>
   </si>
   <si>
     <t>Message authoring status</t>
@@ -446,7 +443,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,12 +468,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -490,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -516,9 +507,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -844,7 +832,7 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -881,10 +869,10 @@
         <v>87</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>89</v>
@@ -912,7 +900,7 @@
       <c r="F2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H2" s="7" t="s">
@@ -942,7 +930,7 @@
       <c r="F4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H4" s="7" t="s">
@@ -970,7 +958,7 @@
       <c r="F6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H6" s="7" t="s">
@@ -1022,7 +1010,7 @@
       <c r="F10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H10" s="7" t="s">
@@ -1036,7 +1024,7 @@
       <c r="F11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H11" s="7" t="s">
@@ -1050,7 +1038,7 @@
       <c r="F12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H12" s="7" t="s">
@@ -1064,7 +1052,7 @@
       <c r="F13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H13" s="7" t="s">
@@ -1078,7 +1066,7 @@
       <c r="F14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H14" s="7" t="s">
@@ -1108,7 +1096,7 @@
       <c r="F16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H16" s="7" t="s">
@@ -1137,7 +1125,7 @@
       <c r="F18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H18" s="7" t="s">
@@ -1166,7 +1154,7 @@
       <c r="F20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H20" s="7" t="s">
@@ -1180,7 +1168,7 @@
       <c r="F21" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H21" s="7" t="s">
@@ -1194,7 +1182,7 @@
       <c r="F22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H22" s="7" t="s">
@@ -1223,7 +1211,7 @@
       <c r="F24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H24" s="7" t="s">
@@ -1237,7 +1225,7 @@
       <c r="F25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H25" s="7" t="s">
@@ -1266,7 +1254,7 @@
       <c r="F27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H27" s="7" t="s">
@@ -1280,7 +1268,7 @@
       <c r="F28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H28" s="7" t="s">
@@ -1306,7 +1294,7 @@
       <c r="F30" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H30" s="7" t="s">
@@ -1320,7 +1308,7 @@
       <c r="F31" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H31" s="7" t="s">
@@ -1349,7 +1337,7 @@
       <c r="F33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H33" s="7" t="s">
@@ -1378,7 +1366,7 @@
       <c r="F35" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="G35" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H35" s="7" t="s">
@@ -1392,7 +1380,7 @@
       <c r="F36" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H36" s="7" t="s">
@@ -1418,7 +1406,7 @@
       <c r="F38" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H38" s="7" t="s">
@@ -1447,7 +1435,7 @@
       <c r="F40" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G40" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H40" s="7" t="s">
@@ -1473,7 +1461,7 @@
       <c r="F42" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H42" s="7" t="s">
@@ -1500,7 +1488,7 @@
       <c r="F44" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G44" s="14" t="s">
+      <c r="G44" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H44" s="7" t="s">
@@ -1514,7 +1502,7 @@
       <c r="F45" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="G45" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H45" s="7" t="s">
@@ -1557,7 +1545,7 @@
       <c r="F48" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G48" s="14" t="s">
+      <c r="G48" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H48" s="7" t="s">
@@ -1574,7 +1562,7 @@
       <c r="F49" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G49" s="14" t="s">
+      <c r="G49" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H49" s="7" t="s">
@@ -1591,7 +1579,7 @@
       <c r="F50" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G50" s="14" t="s">
+      <c r="G50" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H50" s="7" t="s">
@@ -1620,7 +1608,7 @@
       <c r="F52" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G52" s="14" t="s">
+      <c r="G52" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H52" s="7" t="s">
@@ -1646,7 +1634,7 @@
       <c r="F54" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G54" s="14" t="s">
+      <c r="G54" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H54" s="7" t="s">
@@ -1660,7 +1648,7 @@
       <c r="F55" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="G55" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H55" s="7" t="s">
@@ -1686,7 +1674,7 @@
       <c r="F57" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G57" s="14" t="s">
+      <c r="G57" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H57" s="7" t="s">
@@ -1709,7 +1697,7 @@
       <c r="F59" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G59" s="14" t="s">
+      <c r="G59" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H59" s="7" t="s">
@@ -1719,8 +1707,8 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F60" s="1"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
@@ -1741,7 +1729,7 @@
       <c r="F61" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G61" s="14" t="s">
+      <c r="G61" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H61" s="7" t="s">
@@ -1774,10 +1762,10 @@
         <v>24</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H63" s="13" t="s">
-        <v>118</v>
+        <v>88</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
@@ -1799,7 +1787,7 @@
       <c r="F65" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G65" s="14" t="s">
+      <c r="G65" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H65" s="7" t="s">
@@ -1825,7 +1813,7 @@
       <c r="F67" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G67" s="14" t="s">
+      <c r="G67" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H67" s="7" t="s">
@@ -1851,7 +1839,7 @@
       <c r="F69" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G69" s="14" t="s">
+      <c r="G69" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H69" s="7" t="s">
@@ -1863,8 +1851,8 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F70" s="1"/>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
       <c r="I70" s="11"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -1886,7 +1874,7 @@
       <c r="F71" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G71" s="14" t="s">
+      <c r="G71" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H71" s="7" t="s">

</xml_diff>

<commit_message>
Provide messages for SARIF2011.ProvideContextRegion. (#1980)
</commit_message>
<xml_diff>
--- a/docs/Rule factoring.xlsx
+++ b/docs/Rule factoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sarif-sdk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DD2164-FE87-4C44-8B24-B0B2E66C184C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F7FAC9-0971-4894-927F-B3F7EA8F1BE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{6D92DE99-205D-4031-B531-BC3EC8199F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="120">
   <si>
     <t>UrisMustConformToRfc3986</t>
   </si>
@@ -387,9 +387,6 @@
   </si>
   <si>
     <t>ExpressResultLocationsRelativeToMappedTo</t>
-  </si>
-  <si>
-    <t>TODO</t>
   </si>
   <si>
     <t>Message authoring status</t>
@@ -446,7 +443,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,12 +468,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -490,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -516,9 +507,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -844,7 +832,7 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -881,10 +869,10 @@
         <v>87</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>89</v>
@@ -912,7 +900,7 @@
       <c r="F2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H2" s="7" t="s">
@@ -942,7 +930,7 @@
       <c r="F4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H4" s="7" t="s">
@@ -970,7 +958,7 @@
       <c r="F6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H6" s="7" t="s">
@@ -1022,7 +1010,7 @@
       <c r="F10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H10" s="7" t="s">
@@ -1036,7 +1024,7 @@
       <c r="F11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H11" s="7" t="s">
@@ -1050,7 +1038,7 @@
       <c r="F12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H12" s="7" t="s">
@@ -1064,7 +1052,7 @@
       <c r="F13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H13" s="7" t="s">
@@ -1078,7 +1066,7 @@
       <c r="F14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H14" s="7" t="s">
@@ -1108,7 +1096,7 @@
       <c r="F16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H16" s="7" t="s">
@@ -1137,7 +1125,7 @@
       <c r="F18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H18" s="7" t="s">
@@ -1166,7 +1154,7 @@
       <c r="F20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H20" s="7" t="s">
@@ -1180,7 +1168,7 @@
       <c r="F21" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H21" s="7" t="s">
@@ -1194,7 +1182,7 @@
       <c r="F22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H22" s="7" t="s">
@@ -1223,7 +1211,7 @@
       <c r="F24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H24" s="7" t="s">
@@ -1237,7 +1225,7 @@
       <c r="F25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H25" s="7" t="s">
@@ -1266,7 +1254,7 @@
       <c r="F27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H27" s="7" t="s">
@@ -1280,7 +1268,7 @@
       <c r="F28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H28" s="7" t="s">
@@ -1306,7 +1294,7 @@
       <c r="F30" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H30" s="7" t="s">
@@ -1320,7 +1308,7 @@
       <c r="F31" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H31" s="7" t="s">
@@ -1349,7 +1337,7 @@
       <c r="F33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H33" s="7" t="s">
@@ -1378,7 +1366,7 @@
       <c r="F35" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="G35" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H35" s="7" t="s">
@@ -1392,7 +1380,7 @@
       <c r="F36" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H36" s="7" t="s">
@@ -1418,7 +1406,7 @@
       <c r="F38" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H38" s="7" t="s">
@@ -1447,7 +1435,7 @@
       <c r="F40" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G40" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H40" s="7" t="s">
@@ -1473,7 +1461,7 @@
       <c r="F42" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H42" s="7" t="s">
@@ -1500,7 +1488,7 @@
       <c r="F44" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G44" s="14" t="s">
+      <c r="G44" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H44" s="7" t="s">
@@ -1514,7 +1502,7 @@
       <c r="F45" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="G45" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H45" s="7" t="s">
@@ -1557,7 +1545,7 @@
       <c r="F48" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G48" s="14" t="s">
+      <c r="G48" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H48" s="7" t="s">
@@ -1574,7 +1562,7 @@
       <c r="F49" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G49" s="14" t="s">
+      <c r="G49" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H49" s="7" t="s">
@@ -1591,7 +1579,7 @@
       <c r="F50" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G50" s="14" t="s">
+      <c r="G50" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H50" s="7" t="s">
@@ -1620,7 +1608,7 @@
       <c r="F52" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G52" s="14" t="s">
+      <c r="G52" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H52" s="7" t="s">
@@ -1646,7 +1634,7 @@
       <c r="F54" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G54" s="14" t="s">
+      <c r="G54" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H54" s="7" t="s">
@@ -1660,7 +1648,7 @@
       <c r="F55" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="G55" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H55" s="7" t="s">
@@ -1686,7 +1674,7 @@
       <c r="F57" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G57" s="14" t="s">
+      <c r="G57" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H57" s="7" t="s">
@@ -1709,7 +1697,7 @@
       <c r="F59" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G59" s="14" t="s">
+      <c r="G59" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H59" s="7" t="s">
@@ -1719,8 +1707,8 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F60" s="1"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
@@ -1741,7 +1729,7 @@
       <c r="F61" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G61" s="14" t="s">
+      <c r="G61" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H61" s="7" t="s">
@@ -1774,10 +1762,10 @@
         <v>24</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H63" s="13" t="s">
-        <v>118</v>
+        <v>88</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
@@ -1799,7 +1787,7 @@
       <c r="F65" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G65" s="14" t="s">
+      <c r="G65" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H65" s="7" t="s">
@@ -1825,7 +1813,7 @@
       <c r="F67" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G67" s="14" t="s">
+      <c r="G67" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H67" s="7" t="s">
@@ -1851,7 +1839,7 @@
       <c r="F69" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G69" s="14" t="s">
+      <c r="G69" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H69" s="7" t="s">
@@ -1863,8 +1851,8 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F70" s="1"/>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
       <c r="I70" s="11"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -1886,7 +1874,7 @@
       <c r="F71" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G71" s="14" t="s">
+      <c r="G71" s="13" t="s">
         <v>88</v>
       </c>
       <c r="H71" s="7" t="s">

</xml_diff>